<commit_message>
added example code to notebooks
</commit_message>
<xml_diff>
--- a/results/results_corrs/mega_matrix/071921/mega_matrix_corrs_072121.xlsx
+++ b/results/results_corrs/mega_matrix/071921/mega_matrix_corrs_072121.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhec8\Documents\Northwestern_SROP\AUT-Scoring\results\results_corrs\mega_matrix\071921\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7D2CEAD9-CD0A-41B5-ACE2-6419A1563947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BC3BEE-9270-4988-8FDA-6EE5720A4030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2460" windowWidth="21480" windowHeight="11490"/>
+    <workbookView xWindow="-23640" yWindow="2475" windowWidth="21480" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mega_matrix_corrs_071921" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>Variable</t>
   </si>
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1124,11 +1124,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,8 +1493,8 @@
       <c r="C12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1">
-        <v>0.48</v>
+      <c r="D12" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E12" s="1">
         <v>0.19</v>

</xml_diff>